<commit_message>
Added DAC connection util class, still a WIP. Is currently being used to test command effect and response value. Its intended purpose is as a library to be used in DACCurrentStep.py to communicate with the DAC
</commit_message>
<xml_diff>
--- a/DAC_Linearity.xlsx
+++ b/DAC_Linearity.xlsx
@@ -5,16 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fvtuser13782\Desktop\Gitrepos\My_Stuff\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fvtuser13782\Desktop\Gitrepos\DAC_Repo\DAC_Linearity_Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19291E0C-5C5A-40AB-8052-57A5D89B8C94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE9093C2-5B59-4EC3-A8BD-28B7002B8E0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{E6E31D39-7630-41BF-9F2A-9DC60C42B9A3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E6E31D39-7630-41BF-9F2A-9DC60C42B9A3}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Main" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,12 +36,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>DAC Val</t>
-  </si>
-  <si>
-    <t>…</t>
   </si>
   <si>
     <t xml:space="preserve">Red </t>
@@ -90,7 +86,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -108,33 +104,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -188,32 +162,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right/>
       <top style="thin">
         <color indexed="64"/>
@@ -227,20 +175,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -556,130 +500,6 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C254317-2DA8-4585-B54D-118C3AF3F57F}">
-  <dimension ref="C2:I10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="2" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C2" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-    </row>
-    <row r="3" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C3" s="12"/>
-      <c r="D3" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
-    </row>
-    <row r="4" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C4" s="12"/>
-      <c r="D4" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="I4" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C5" s="8">
-        <v>0</v>
-      </c>
-      <c r="D5" s="1"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="1"/>
-      <c r="I5" s="3"/>
-    </row>
-    <row r="6" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C6" s="9">
-        <v>1</v>
-      </c>
-      <c r="D6" s="1"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="1"/>
-      <c r="I6" s="2"/>
-    </row>
-    <row r="7" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C7" s="9">
-        <v>2</v>
-      </c>
-      <c r="D7" s="1"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="1"/>
-      <c r="I7" s="2"/>
-    </row>
-    <row r="8" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C8" s="9">
-        <v>3</v>
-      </c>
-      <c r="D8" s="1"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="1"/>
-      <c r="I8" s="2"/>
-    </row>
-    <row r="9" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C9" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="D9" s="1"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="1"/>
-      <c r="I9" s="2"/>
-    </row>
-    <row r="10" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C10" s="10">
-        <v>1023</v>
-      </c>
-      <c r="D10" s="4"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="6"/>
-    </row>
-  </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="G3:I3"/>
-    <mergeCell ref="D2:I2"/>
-    <mergeCell ref="C2:C4"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBD8FA61-ABFA-4BAB-984B-C741CC0DB7B1}">
   <dimension ref="A1:H1027"/>
   <sheetViews>
@@ -690,50 +510,50 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="8"/>
+      <c r="B2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="8"/>
+      <c r="B3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="12"/>
-      <c r="B3" s="7" t="s">
+      <c r="F3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="7" t="s">
+      <c r="G3" s="6" t="s">
         <v>8</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -742,27 +562,27 @@
       </c>
       <c r="B4" s="1">
         <f ca="1">RAND()*30</f>
-        <v>13.053509232228752</v>
+        <v>6.8199673694543925</v>
       </c>
       <c r="C4" s="1">
         <f t="shared" ref="C4:G19" ca="1" si="0">RAND()*30</f>
-        <v>7.1794495460386063</v>
+        <v>0.62715517076154415</v>
       </c>
       <c r="D4" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>2.0877121690684373</v>
+        <v>11.907618197763471</v>
       </c>
       <c r="E4" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>10.660659903647009</v>
+        <v>13.274234427603993</v>
       </c>
       <c r="F4" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4.4905119967547646</v>
+        <v>14.148061074208508</v>
       </c>
       <c r="G4" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>23.851614792178356</v>
+        <v>2.302099672844701</v>
       </c>
       <c r="H4" s="1"/>
     </row>
@@ -772,27 +592,27 @@
       </c>
       <c r="B5" s="1">
         <f t="shared" ref="B5:G20" ca="1" si="1">RAND()*30</f>
-        <v>8.0672705683624297</v>
+        <v>8.0241290075402567</v>
       </c>
       <c r="C5" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>22.78784885655789</v>
+        <v>10.021644652454606</v>
       </c>
       <c r="D5" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>10.156541899981006</v>
+        <v>7.3882466306190828</v>
       </c>
       <c r="E5" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>27.118914672733759</v>
+        <v>28.178548796557955</v>
       </c>
       <c r="F5" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>9.5199266121486019</v>
+        <v>20.302049912079461</v>
       </c>
       <c r="G5" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>25.870794483517205</v>
+        <v>4.1619536151320542</v>
       </c>
       <c r="H5" s="1"/>
     </row>
@@ -802,27 +622,27 @@
       </c>
       <c r="B6" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>20.797687784696926</v>
+        <v>27.958997394993592</v>
       </c>
       <c r="C6" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>0.93232476230390326</v>
+        <v>29.396466737134336</v>
       </c>
       <c r="D6" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>28.557511815353642</v>
+        <v>24.868312507198393</v>
       </c>
       <c r="E6" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>19.03154744269786</v>
+        <v>4.3752753205036532</v>
       </c>
       <c r="F6" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>11.786229147617345</v>
+        <v>11.635566650146183</v>
       </c>
       <c r="G6" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>9.3885394824774195</v>
+        <v>29.304790849664066</v>
       </c>
       <c r="H6" s="1"/>
     </row>
@@ -832,27 +652,27 @@
       </c>
       <c r="B7" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>25.005358198849599</v>
+        <v>7.6616244858983551E-2</v>
       </c>
       <c r="C7" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4.9440019143362148</v>
+        <v>2.1989363962650819</v>
       </c>
       <c r="D7" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>13.309645059232778</v>
+        <v>10.324169607100819</v>
       </c>
       <c r="E7" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>8.9679733185199293</v>
+        <v>12.140718981327586</v>
       </c>
       <c r="F7" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>11.709200825693522</v>
+        <v>14.830662303951863</v>
       </c>
       <c r="G7" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>23.670599064281802</v>
+        <v>7.9276345954205221</v>
       </c>
       <c r="H7" s="1"/>
     </row>
@@ -862,27 +682,27 @@
       </c>
       <c r="B8" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>16.424659279079531</v>
+        <v>5.5097933521044142</v>
       </c>
       <c r="C8" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>0.76708421214409017</v>
+        <v>26.024107715295816</v>
       </c>
       <c r="D8" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>16.065490433526143</v>
+        <v>22.883789066167921</v>
       </c>
       <c r="E8" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>21.496437761734462</v>
+        <v>5.1348494511393099</v>
       </c>
       <c r="F8" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>21.78747801901828</v>
+        <v>6.2916507857076933</v>
       </c>
       <c r="G8" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>10.06310708929424</v>
+        <v>0.82605559063585021</v>
       </c>
       <c r="H8" s="1"/>
     </row>
@@ -892,27 +712,27 @@
       </c>
       <c r="B9" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>15.464031480848513</v>
+        <v>18.023325332165275</v>
       </c>
       <c r="C9" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>2.0546068961170083</v>
+        <v>12.653119217648605</v>
       </c>
       <c r="D9" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3.5779251511544441</v>
+        <v>24.049303929078118</v>
       </c>
       <c r="E9" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>7.4631665746700184</v>
+        <v>20.416608475260329</v>
       </c>
       <c r="F9" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>17.363527139082304</v>
+        <v>26.000828072615427</v>
       </c>
       <c r="G9" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>22.295256072911879</v>
+        <v>22.712203762742842</v>
       </c>
       <c r="H9" s="1"/>
     </row>
@@ -922,27 +742,27 @@
       </c>
       <c r="B10" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3.0967723964710716</v>
+        <v>3.1834600716408734</v>
       </c>
       <c r="C10" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>24.177977416906071</v>
+        <v>7.7720157884993775</v>
       </c>
       <c r="D10" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>29.632870145977577</v>
+        <v>1.0873135829749569</v>
       </c>
       <c r="E10" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>18.139151842310568</v>
+        <v>12.471578893529454</v>
       </c>
       <c r="F10" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4.2051197391765873</v>
+        <v>12.793041572402643</v>
       </c>
       <c r="G10" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>17.010140960541925</v>
+        <v>16.069325546778963</v>
       </c>
       <c r="H10" s="1"/>
     </row>
@@ -952,27 +772,27 @@
       </c>
       <c r="B11" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>21.566736900997078</v>
+        <v>10.099842463685833</v>
       </c>
       <c r="C11" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>2.7449502290332495</v>
+        <v>10.439797985883564</v>
       </c>
       <c r="D11" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>15.696939484588192</v>
+        <v>28.409605843359053</v>
       </c>
       <c r="E11" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>19.400891818469443</v>
+        <v>26.383320766559535</v>
       </c>
       <c r="F11" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>16.84767236124128</v>
+        <v>10.759648679253139</v>
       </c>
       <c r="G11" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>20.026220133869817</v>
+        <v>23.183925178829064</v>
       </c>
       <c r="H11" s="1"/>
     </row>
@@ -982,27 +802,27 @@
       </c>
       <c r="B12" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>14.538277881528618</v>
+        <v>17.397540349458559</v>
       </c>
       <c r="C12" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>28.59185032559359</v>
+        <v>27.958081865285422</v>
       </c>
       <c r="D12" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>22.878205509850176</v>
+        <v>13.716420023277147</v>
       </c>
       <c r="E12" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>6.3723166191131186</v>
+        <v>7.6409185603608822</v>
       </c>
       <c r="F12" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4.5844281458158882</v>
+        <v>0.50129876339978452</v>
       </c>
       <c r="G12" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>24.21868314383455</v>
+        <v>2.28901278387844</v>
       </c>
       <c r="H12" s="1"/>
     </row>
@@ -1012,27 +832,27 @@
       </c>
       <c r="B13" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>16.252105745870171</v>
+        <v>26.948806983828671</v>
       </c>
       <c r="C13" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>13.192297159323234</v>
+        <v>17.914971809953997</v>
       </c>
       <c r="D13" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>16.578715480449741</v>
+        <v>13.29284514539254</v>
       </c>
       <c r="E13" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>13.871902546122669</v>
+        <v>1.6737225476416007</v>
       </c>
       <c r="F13" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>12.545186080559358</v>
+        <v>16.541339951156495</v>
       </c>
       <c r="G13" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>16.015959137096324</v>
+        <v>13.842329479622462</v>
       </c>
       <c r="H13" s="1"/>
     </row>
@@ -1042,27 +862,27 @@
       </c>
       <c r="B14" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>10.013822507063868</v>
+        <v>7.0852319604494705</v>
       </c>
       <c r="C14" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>15.328333096237397</v>
+        <v>22.842851589850852</v>
       </c>
       <c r="D14" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>8.013886609964505</v>
+        <v>7.3444247246896124</v>
       </c>
       <c r="E14" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>13.615893858779909</v>
+        <v>25.14127424160538</v>
       </c>
       <c r="F14" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>15.860818778585386</v>
+        <v>8.7491445755227399</v>
       </c>
       <c r="G14" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>29.581918148127489</v>
+        <v>3.9297753326707197</v>
       </c>
       <c r="H14" s="1"/>
     </row>
@@ -1072,27 +892,27 @@
       </c>
       <c r="B15" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>25.638749085065832</v>
+        <v>21.08974851869668</v>
       </c>
       <c r="C15" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>2.9844975407507137</v>
+        <v>13.15808341120116</v>
       </c>
       <c r="D15" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>25.93108585219025</v>
+        <v>7.7018903169134507</v>
       </c>
       <c r="E15" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>8.2763843535710313E-2</v>
+        <v>6.3629542981415881</v>
       </c>
       <c r="F15" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>25.235307131757708</v>
+        <v>21.812859663478246</v>
       </c>
       <c r="G15" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>17.981769933650334</v>
+        <v>29.807053380276653</v>
       </c>
       <c r="H15" s="1"/>
     </row>
@@ -1102,27 +922,27 @@
       </c>
       <c r="B16" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>27.915108754243636</v>
+        <v>6.7733540618734338</v>
       </c>
       <c r="C16" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>5.2883075037103122</v>
+        <v>7.5448653672915462</v>
       </c>
       <c r="D16" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>6.1996445330321759</v>
+        <v>26.459786792441847</v>
       </c>
       <c r="E16" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4.8473390107723304</v>
+        <v>9.9984169635958011</v>
       </c>
       <c r="F16" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>19.892335027693353</v>
+        <v>25.871461596609493</v>
       </c>
       <c r="G16" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>9.2184674761298862</v>
+        <v>16.123655312634611</v>
       </c>
       <c r="H16" s="1"/>
     </row>
@@ -1132,27 +952,27 @@
       </c>
       <c r="B17" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>9.9526891664442889</v>
+        <v>0.69671645731336329</v>
       </c>
       <c r="C17" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>19.805166873436107</v>
+        <v>19.624315196683948</v>
       </c>
       <c r="D17" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>21.756432638170136</v>
+        <v>27.051701668242309</v>
       </c>
       <c r="E17" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>15.917610096432867</v>
+        <v>5.7892214130153672</v>
       </c>
       <c r="F17" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>15.960455658188305</v>
+        <v>1.2359603346089054</v>
       </c>
       <c r="G17" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>14.753460320275638</v>
+        <v>22.650476570337517</v>
       </c>
       <c r="H17" s="1"/>
     </row>
@@ -1162,27 +982,27 @@
       </c>
       <c r="B18" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>13.608979018151475</v>
+        <v>19.186653275450446</v>
       </c>
       <c r="C18" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>24.950465637771632</v>
+        <v>12.977742207226594</v>
       </c>
       <c r="D18" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3.9642175359573075</v>
+        <v>3.9091443878939671</v>
       </c>
       <c r="E18" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>8.388927801826032</v>
+        <v>11.575063012307449</v>
       </c>
       <c r="F18" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>24.849606677688605</v>
+        <v>23.695098358745181</v>
       </c>
       <c r="G18" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3.9703175145076655</v>
+        <v>25.962051212456654</v>
       </c>
       <c r="H18" s="1"/>
     </row>
@@ -1192,27 +1012,27 @@
       </c>
       <c r="B19" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>24.39317240584818</v>
+        <v>25.766110175694308</v>
       </c>
       <c r="C19" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>6.2339547604276779</v>
+        <v>15.819575200823925</v>
       </c>
       <c r="D19" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4.6563274323461439</v>
+        <v>29.99373669931062</v>
       </c>
       <c r="E19" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4.2337717137539261</v>
+        <v>9.9670584822966042</v>
       </c>
       <c r="F19" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>11.105138270905782</v>
+        <v>22.847647307006941</v>
       </c>
       <c r="G19" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1.6960454919205703</v>
+        <v>29.181868399976089</v>
       </c>
       <c r="H19" s="1"/>
     </row>
@@ -1222,27 +1042,27 @@
       </c>
       <c r="B20" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>8.6157278798712138</v>
+        <v>4.85664992826994</v>
       </c>
       <c r="C20" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>28.709502074488586</v>
+        <v>15.436173945040203</v>
       </c>
       <c r="D20" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>21.157292433397451</v>
+        <v>27.151903057439707</v>
       </c>
       <c r="E20" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>20.362302816239271</v>
+        <v>4.5829928572196179</v>
       </c>
       <c r="F20" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>24.714408333239259</v>
+        <v>29.537131499663577</v>
       </c>
       <c r="G20" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1.4181604552209937</v>
+        <v>16.067200481256432</v>
       </c>
       <c r="H20" s="1"/>
     </row>
@@ -1252,27 +1072,27 @@
       </c>
       <c r="B21" s="1">
         <f t="shared" ref="B21:G36" ca="1" si="2">RAND()*30</f>
-        <v>2.8170724728128937</v>
+        <v>28.000249469481087</v>
       </c>
       <c r="C21" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>2.7371331994763173</v>
+        <v>13.355302108002382</v>
       </c>
       <c r="D21" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>7.8844628739254299</v>
+        <v>29.19334775334163</v>
       </c>
       <c r="E21" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>12.330692453611265</v>
+        <v>2.5135199309454634</v>
       </c>
       <c r="F21" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>19.512981497338131</v>
+        <v>21.124581055027264</v>
       </c>
       <c r="G21" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>12.354340162103256</v>
+        <v>4.1383212154714419</v>
       </c>
       <c r="H21" s="1"/>
     </row>
@@ -1282,27 +1102,27 @@
       </c>
       <c r="B22" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>16.258370938642237</v>
+        <v>19.777359978683826</v>
       </c>
       <c r="C22" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>12.500794566840502</v>
+        <v>18.845107470356314</v>
       </c>
       <c r="D22" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>17.158767940068682</v>
+        <v>17.282128125069818</v>
       </c>
       <c r="E22" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>27.017642151361791</v>
+        <v>8.2798625155502634</v>
       </c>
       <c r="F22" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>21.620174317687301</v>
+        <v>10.720336586959062</v>
       </c>
       <c r="G22" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>20.778973811525375</v>
+        <v>23.53798317546125</v>
       </c>
       <c r="H22" s="1"/>
     </row>
@@ -1312,27 +1132,27 @@
       </c>
       <c r="B23" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>4.8082054376542613</v>
+        <v>16.365711256137931</v>
       </c>
       <c r="C23" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>9.5990523725583792</v>
+        <v>24.497814656322806</v>
       </c>
       <c r="D23" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>27.303928591307518</v>
+        <v>16.744395836678528</v>
       </c>
       <c r="E23" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>26.855443868736074</v>
+        <v>14.886639421107501</v>
       </c>
       <c r="F23" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>23.388748986208761</v>
+        <v>20.425628694076334</v>
       </c>
       <c r="G23" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>11.410133782279896</v>
+        <v>6.7900492715525465</v>
       </c>
       <c r="H23" s="1"/>
     </row>
@@ -1342,27 +1162,27 @@
       </c>
       <c r="B24" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>8.3849541532894953</v>
+        <v>25.265280343842853</v>
       </c>
       <c r="C24" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>3.4369573616601459</v>
+        <v>27.034927015699022</v>
       </c>
       <c r="D24" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>29.108011330052186</v>
+        <v>13.291818786134556</v>
       </c>
       <c r="E24" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>29.16221264486099</v>
+        <v>1.0649561819002606</v>
       </c>
       <c r="F24" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>7.0180039710322193</v>
+        <v>19.425878968834649</v>
       </c>
       <c r="G24" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>29.56382091782605</v>
+        <v>17.093154257896995</v>
       </c>
       <c r="H24" s="1"/>
     </row>
@@ -1372,27 +1192,27 @@
       </c>
       <c r="B25" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>17.612877260384256</v>
+        <v>20.319831568526908</v>
       </c>
       <c r="C25" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>12.257023813304821</v>
+        <v>0.3581925649512685</v>
       </c>
       <c r="D25" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>8.2229823220298393</v>
+        <v>10.552488654786105</v>
       </c>
       <c r="E25" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>25.367035259623034</v>
+        <v>4.482698529525285</v>
       </c>
       <c r="F25" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>16.453832879906781</v>
+        <v>16.707131480440264</v>
       </c>
       <c r="G25" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>6.2137674177147968</v>
+        <v>1.4268983296647586</v>
       </c>
       <c r="H25" s="1"/>
     </row>
@@ -1402,27 +1222,27 @@
       </c>
       <c r="B26" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>28.224960206069618</v>
+        <v>13.496670441530817</v>
       </c>
       <c r="C26" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>6.9852235342731817</v>
+        <v>5.8420928370451843</v>
       </c>
       <c r="D26" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>5.654666983351456</v>
+        <v>12.115214359302177</v>
       </c>
       <c r="E26" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>20.674566411460528</v>
+        <v>27.122705970916073</v>
       </c>
       <c r="F26" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>24.237011180955527</v>
+        <v>23.508225242365754</v>
       </c>
       <c r="G26" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>16.731782346857901</v>
+        <v>27.875348573579615</v>
       </c>
       <c r="H26" s="1"/>
     </row>
@@ -1432,27 +1252,27 @@
       </c>
       <c r="B27" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>15.826722241784584</v>
+        <v>10.774115446014614</v>
       </c>
       <c r="C27" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>19.762290094950245</v>
+        <v>8.9562969273492641</v>
       </c>
       <c r="D27" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>22.774927467785119</v>
+        <v>14.329746921234893</v>
       </c>
       <c r="E27" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>27.576274826293204</v>
+        <v>9.8582436106365599</v>
       </c>
       <c r="F27" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>11.76654919361108</v>
+        <v>10.801532573198102</v>
       </c>
       <c r="G27" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>8.8419082584571296</v>
+        <v>1.9441529162782423</v>
       </c>
       <c r="H27" s="1"/>
     </row>
@@ -1462,27 +1282,27 @@
       </c>
       <c r="B28" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>14.447592186497749</v>
+        <v>12.120910454663731</v>
       </c>
       <c r="C28" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>1.4251134809979515</v>
+        <v>19.585984381055226</v>
       </c>
       <c r="D28" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>28.882290548009298</v>
+        <v>13.426666168021983</v>
       </c>
       <c r="E28" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>8.0895178201285507</v>
+        <v>10.377611037322909</v>
       </c>
       <c r="F28" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>17.363416690828483</v>
+        <v>12.9690042761552</v>
       </c>
       <c r="G28" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>16.872413750564746</v>
+        <v>7.8152392738794783</v>
       </c>
       <c r="H28" s="1"/>
     </row>
@@ -1492,27 +1312,27 @@
       </c>
       <c r="B29" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>21.143926907479415</v>
+        <v>11.707035590436618</v>
       </c>
       <c r="C29" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>16.015190728857966</v>
+        <v>6.7600482498779808</v>
       </c>
       <c r="D29" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>11.728509789703699</v>
+        <v>27.137507103266888</v>
       </c>
       <c r="E29" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>25.51395860934678</v>
+        <v>17.624740406088211</v>
       </c>
       <c r="F29" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>27.289067410762556</v>
+        <v>25.439128977638983</v>
       </c>
       <c r="G29" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>5.8462499252538516</v>
+        <v>21.456221541005469</v>
       </c>
       <c r="H29" s="1"/>
     </row>
@@ -1522,27 +1342,27 @@
       </c>
       <c r="B30" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>8.8208715788467096</v>
+        <v>27.59774942883654</v>
       </c>
       <c r="C30" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>9.1745683643248999</v>
+        <v>21.704366269718307</v>
       </c>
       <c r="D30" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>2.4735352429495761</v>
+        <v>2.4762265213101764</v>
       </c>
       <c r="E30" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>26.867780717880702</v>
+        <v>3.1777656134979262</v>
       </c>
       <c r="F30" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>8.6533600088452687</v>
+        <v>19.310546289638008</v>
       </c>
       <c r="G30" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>1.6572474788401581</v>
+        <v>28.077422199361546</v>
       </c>
       <c r="H30" s="1"/>
     </row>
@@ -1552,27 +1372,27 @@
       </c>
       <c r="B31" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>22.763248945469002</v>
+        <v>24.60690615025084</v>
       </c>
       <c r="C31" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>23.935430654467531</v>
+        <v>15.288784941679539</v>
       </c>
       <c r="D31" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>18.988997271646284</v>
+        <v>21.425913031131259</v>
       </c>
       <c r="E31" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>7.6401869588120297</v>
+        <v>11.578488076813938</v>
       </c>
       <c r="F31" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>19.950817653800613</v>
+        <v>17.004151950858581</v>
       </c>
       <c r="G31" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>27.191721105879733</v>
+        <v>22.093898495603426</v>
       </c>
       <c r="H31" s="1"/>
     </row>
@@ -1582,27 +1402,27 @@
       </c>
       <c r="B32" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>1.450073019998771</v>
+        <v>25.647375665408052</v>
       </c>
       <c r="C32" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>10.417814047446615</v>
+        <v>19.247092437205524</v>
       </c>
       <c r="D32" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>11.373907938093131</v>
+        <v>8.5501631275460657</v>
       </c>
       <c r="E32" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>15.365300881059317</v>
+        <v>18.596146336500652</v>
       </c>
       <c r="F32" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>7.7450523336475454</v>
+        <v>6.5542813827554403</v>
       </c>
       <c r="G32" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>29.804080259354745</v>
+        <v>15.530363642611352</v>
       </c>
       <c r="H32" s="1"/>
     </row>
@@ -1612,27 +1432,27 @@
       </c>
       <c r="B33" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>8.6583677917479722</v>
+        <v>22.790603528383272</v>
       </c>
       <c r="C33" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>23.927406159528221</v>
+        <v>6.5748321815465882</v>
       </c>
       <c r="D33" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>17.127105834217545</v>
+        <v>4.8492277214290489</v>
       </c>
       <c r="E33" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>17.632798412412861</v>
+        <v>18.286778208620788</v>
       </c>
       <c r="F33" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>1.0666347955377908</v>
+        <v>25.213486580434619</v>
       </c>
       <c r="G33" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>1.282014279856919</v>
+        <v>25.226251138878961</v>
       </c>
       <c r="H33" s="1"/>
     </row>
@@ -1642,27 +1462,27 @@
       </c>
       <c r="B34" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>17.122338317619597</v>
+        <v>11.19096347670704</v>
       </c>
       <c r="C34" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0.44452842992421915</v>
+        <v>3.1012139231251226</v>
       </c>
       <c r="D34" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>9.3840733366497719</v>
+        <v>13.005471525894469</v>
       </c>
       <c r="E34" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>29.433753077570273</v>
+        <v>0.86154806623042757</v>
       </c>
       <c r="F34" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>1.6893017378469621</v>
+        <v>21.797252197234556</v>
       </c>
       <c r="G34" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>15.737111299713318</v>
+        <v>6.9389728334951792</v>
       </c>
       <c r="H34" s="1"/>
     </row>
@@ -1672,27 +1492,27 @@
       </c>
       <c r="B35" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>5.5409537377193931</v>
+        <v>16.712452671008499</v>
       </c>
       <c r="C35" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>26.470518794851351</v>
+        <v>3.5853596674801835</v>
       </c>
       <c r="D35" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>5.952730581289952</v>
+        <v>1.3123961527210193</v>
       </c>
       <c r="E35" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>13.779131431670095</v>
+        <v>14.625616402720004</v>
       </c>
       <c r="F35" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>29.274335892783352</v>
+        <v>29.93898640345682</v>
       </c>
       <c r="G35" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>26.895213955858999</v>
+        <v>23.091187375725163</v>
       </c>
       <c r="H35" s="1"/>
     </row>
@@ -1702,27 +1522,27 @@
       </c>
       <c r="B36" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>4.7170247337742586</v>
+        <v>9.1774406443154177</v>
       </c>
       <c r="C36" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>21.106199705039373</v>
+        <v>10.371103289198288</v>
       </c>
       <c r="D36" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>3.9730017524800298</v>
+        <v>12.833791875301907</v>
       </c>
       <c r="E36" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>12.521742864677242</v>
+        <v>9.8822513959814327</v>
       </c>
       <c r="F36" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>25.204211310700789</v>
+        <v>16.659749252080566</v>
       </c>
       <c r="G36" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>13.224447981559807</v>
+        <v>15.447477395516076</v>
       </c>
       <c r="H36" s="1"/>
     </row>
@@ -1732,27 +1552,27 @@
       </c>
       <c r="B37" s="1">
         <f t="shared" ref="B37:G50" ca="1" si="3">RAND()*30</f>
-        <v>25.745610538619971</v>
+        <v>22.120812459564348</v>
       </c>
       <c r="C37" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>29.207736438644062</v>
+        <v>1.0422899883765935</v>
       </c>
       <c r="D37" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>15.8395759035701</v>
+        <v>11.870970999516121</v>
       </c>
       <c r="E37" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>2.4276170606233505</v>
+        <v>14.357884747711578</v>
       </c>
       <c r="F37" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.91071980744212411</v>
+        <v>2.1402612586126746</v>
       </c>
       <c r="G37" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>15.785929755422853</v>
+        <v>28.53974444114418</v>
       </c>
       <c r="H37" s="1"/>
     </row>
@@ -1762,27 +1582,27 @@
       </c>
       <c r="B38" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>26.520588482070366</v>
+        <v>1.1029107577398733</v>
       </c>
       <c r="C38" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>13.286516681510236</v>
+        <v>13.655663177586508</v>
       </c>
       <c r="D38" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>4.1528021397459582</v>
+        <v>5.1029373789052643</v>
       </c>
       <c r="E38" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>10.789642451473368</v>
+        <v>17.927308112760169</v>
       </c>
       <c r="F38" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>22.775755912057001</v>
+        <v>13.353871806928662</v>
       </c>
       <c r="G38" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>24.046708845910509</v>
+        <v>3.1867067602112442</v>
       </c>
       <c r="H38" s="1"/>
     </row>
@@ -1792,27 +1612,27 @@
       </c>
       <c r="B39" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>20.52527829506678</v>
+        <v>23.116040973356238</v>
       </c>
       <c r="C39" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>1.8056333319141971</v>
+        <v>16.117570462090669</v>
       </c>
       <c r="D39" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>25.084994854841195</v>
+        <v>13.859582809073348</v>
       </c>
       <c r="E39" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>25.130863379773409</v>
+        <v>10.719873664848452</v>
       </c>
       <c r="F39" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>15.267512169340412</v>
+        <v>18.917445166135714</v>
       </c>
       <c r="G39" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>19.154949218105489</v>
+        <v>25.405284693809044</v>
       </c>
       <c r="H39" s="1"/>
     </row>
@@ -1822,27 +1642,27 @@
       </c>
       <c r="B40" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>28.082717119025396</v>
+        <v>12.536905681500301</v>
       </c>
       <c r="C40" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>15.155115299414286</v>
+        <v>9.5766934988824524</v>
       </c>
       <c r="D40" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>3.8443109628099279</v>
+        <v>11.434292407899861</v>
       </c>
       <c r="E40" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>29.402345165554316</v>
+        <v>25.509190153717515</v>
       </c>
       <c r="F40" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>21.799430850055906</v>
+        <v>4.4423886986711567</v>
       </c>
       <c r="G40" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>4.4743427746205011</v>
+        <v>25.20423971377534</v>
       </c>
       <c r="H40" s="1"/>
     </row>
@@ -1852,27 +1672,27 @@
       </c>
       <c r="B41" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>14.104463180217799</v>
+        <v>0.4630136207368607</v>
       </c>
       <c r="C41" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>5.0552866703840236</v>
+        <v>2.2858648975323517</v>
       </c>
       <c r="D41" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>1.1331505459331115</v>
+        <v>6.5397795909745646</v>
       </c>
       <c r="E41" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>17.96371746032888</v>
+        <v>12.10039067152605</v>
       </c>
       <c r="F41" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>4.3357210418684549</v>
+        <v>29.217574847306722</v>
       </c>
       <c r="G41" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>5.7947551258769963</v>
+        <v>11.478783776849554</v>
       </c>
       <c r="H41" s="1"/>
     </row>
@@ -1882,27 +1702,27 @@
       </c>
       <c r="B42" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>19.121789199524912</v>
+        <v>8.6277146427597788</v>
       </c>
       <c r="C42" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>14.620971775284916</v>
+        <v>2.2808894226325362</v>
       </c>
       <c r="D42" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>15.465815504611689</v>
+        <v>23.731021152058325</v>
       </c>
       <c r="E42" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>9.2094215850960985</v>
+        <v>2.1785677709080389</v>
       </c>
       <c r="F42" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>19.161243588017847</v>
+        <v>15.151309019327014</v>
       </c>
       <c r="G42" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>27.152353077090442</v>
+        <v>11.862369417092619</v>
       </c>
       <c r="H42" s="1"/>
     </row>
@@ -1912,27 +1732,27 @@
       </c>
       <c r="B43" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>9.1827465381563318</v>
+        <v>28.485674355969554</v>
       </c>
       <c r="C43" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>14.58920751036333</v>
+        <v>18.09120534126922</v>
       </c>
       <c r="D43" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>28.625358965163464</v>
+        <v>21.440271246535485</v>
       </c>
       <c r="E43" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>9.1334226967310936</v>
+        <v>7.3238947123793272</v>
       </c>
       <c r="F43" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>7.5506452392336847</v>
+        <v>13.726940214320111</v>
       </c>
       <c r="G43" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>27.932350925248379</v>
+        <v>24.661744296613104</v>
       </c>
       <c r="H43" s="1"/>
     </row>
@@ -1942,27 +1762,27 @@
       </c>
       <c r="B44" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>23.275110082101619</v>
+        <v>26.726764142710874</v>
       </c>
       <c r="C44" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>21.54544183583311</v>
+        <v>10.608738917305171</v>
       </c>
       <c r="D44" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>2.5315766808711535</v>
+        <v>28.986923314853115</v>
       </c>
       <c r="E44" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>5.5726351889423231</v>
+        <v>2.0580086026027566</v>
       </c>
       <c r="F44" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>26.198178672311599</v>
+        <v>5.1771274437548058</v>
       </c>
       <c r="G44" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>11.965222938347228</v>
+        <v>15.931548479018497</v>
       </c>
       <c r="H44" s="1"/>
     </row>
@@ -1972,27 +1792,27 @@
       </c>
       <c r="B45" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>10.239796607135121</v>
+        <v>3.8594750711108814</v>
       </c>
       <c r="C45" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>28.138983835860742</v>
+        <v>23.504893191072757</v>
       </c>
       <c r="D45" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>19.029789073719233</v>
+        <v>13.776275450227216</v>
       </c>
       <c r="E45" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>19.676002409335112</v>
+        <v>24.776999091410847</v>
       </c>
       <c r="F45" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>22.574653748791718</v>
+        <v>14.615828334599454</v>
       </c>
       <c r="G45" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>21.00744937792895</v>
+        <v>19.956666016719581</v>
       </c>
       <c r="H45" s="1"/>
     </row>
@@ -2002,27 +1822,27 @@
       </c>
       <c r="B46" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>11.589140417171183</v>
+        <v>20.09575063000802</v>
       </c>
       <c r="C46" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>18.753544078738074</v>
+        <v>0.18144268198238112</v>
       </c>
       <c r="D46" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0.21467422959370541</v>
+        <v>19.779916747656394</v>
       </c>
       <c r="E46" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>23.652857447377524</v>
+        <v>5.9982133961547222</v>
       </c>
       <c r="F46" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>18.771161356530801</v>
+        <v>6.765723837183466</v>
       </c>
       <c r="G46" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>19.883740751624639</v>
+        <v>27.752313867964425</v>
       </c>
       <c r="H46" s="1"/>
     </row>
@@ -2032,27 +1852,27 @@
       </c>
       <c r="B47" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>5.412657325435239</v>
+        <v>10.485651275796773</v>
       </c>
       <c r="C47" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>23.422664965003523</v>
+        <v>14.211713058781271</v>
       </c>
       <c r="D47" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>3.4923747696093344</v>
+        <v>5.260981830004039</v>
       </c>
       <c r="E47" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>29.03955868633513</v>
+        <v>0.63702218509967712</v>
       </c>
       <c r="F47" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>25.139909488134691</v>
+        <v>15.318016897475143</v>
       </c>
       <c r="G47" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>19.421613315768443</v>
+        <v>4.2737036283415542</v>
       </c>
       <c r="H47" s="1"/>
     </row>
@@ -2062,27 +1882,27 @@
       </c>
       <c r="B48" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>18.083397497277719</v>
+        <v>16.288198075162573</v>
       </c>
       <c r="C48" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>17.874784230800771</v>
+        <v>24.415538631382145</v>
       </c>
       <c r="D48" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>25.942612748108203</v>
+        <v>6.5733519037057011</v>
       </c>
       <c r="E48" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>17.372903273730863</v>
+        <v>20.336770254862699</v>
       </c>
       <c r="F48" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>13.679967453742734</v>
+        <v>22.538743979004622</v>
       </c>
       <c r="G48" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>24.146101332375842</v>
+        <v>16.59204529715424</v>
       </c>
       <c r="H48" s="1"/>
     </row>
@@ -2092,27 +1912,27 @@
       </c>
       <c r="B49" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>24.699249483261745</v>
+        <v>27.054422168003615</v>
       </c>
       <c r="C49" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>6.285376991298123</v>
+        <v>2.6541342568671911</v>
       </c>
       <c r="D49" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>18.893001283766512</v>
+        <v>28.351108517312266</v>
       </c>
       <c r="E49" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>7.2174456144895096</v>
+        <v>26.162228771024928</v>
       </c>
       <c r="F49" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>6.7865047418753877</v>
+        <v>10.451073222652486</v>
       </c>
       <c r="G49" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>26.630805405323827</v>
+        <v>0.39526502113181983</v>
       </c>
       <c r="H49" s="1"/>
     </row>
@@ -2122,27 +1942,27 @@
       </c>
       <c r="B50" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>12.705119401461515</v>
+        <v>24.727495769627641</v>
       </c>
       <c r="C50" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>29.696425925620982</v>
+        <v>27.287248222867078</v>
       </c>
       <c r="D50" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>29.405058769633666</v>
+        <v>25.142930025189251</v>
       </c>
       <c r="E50" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>5.4871906073078929</v>
+        <v>12.192220622816755</v>
       </c>
       <c r="F50" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>16.377406700803736</v>
+        <v>27.393726331342819</v>
       </c>
       <c r="G50" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>21.585638193087675</v>
+        <v>29.290206993845626</v>
       </c>
       <c r="H50" s="1"/>
     </row>
@@ -8979,15 +8799,15 @@
       <c r="H1026" s="1"/>
     </row>
     <row r="1027" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1027" s="6">
+      <c r="A1027" s="5">
         <v>1023</v>
       </c>
-      <c r="B1027" s="5"/>
-      <c r="C1027" s="5"/>
-      <c r="D1027" s="5"/>
-      <c r="E1027" s="4"/>
-      <c r="F1027" s="5"/>
-      <c r="G1027" s="6"/>
+      <c r="B1027" s="4"/>
+      <c r="C1027" s="4"/>
+      <c r="D1027" s="4"/>
+      <c r="E1027" s="3"/>
+      <c r="F1027" s="4"/>
+      <c r="G1027" s="5"/>
       <c r="H1027" s="1"/>
     </row>
   </sheetData>

</xml_diff>